<commit_message>
Actualizar documentación de análisis de riesgos
</commit_message>
<xml_diff>
--- a/documentation/Analsis_de_Riesgos_GrupoA.xlsx
+++ b/documentation/Analsis_de_Riesgos_GrupoA.xlsx
@@ -5,36 +5,23 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universidad\Octavo Semestre\Software Seguro\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Det-Pc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7185922-C7DF-4D68-9FCC-3296F3AE59ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DC37BB-4D2E-4919-9DDA-A4EC2C253EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registro de Riesgos" sheetId="1" r:id="rId1"/>
     <sheet name="Referencias" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>Número de Riesgo</t>
   </si>
@@ -69,9 +56,6 @@
     <t>Alto (3)</t>
   </si>
   <si>
-    <t>Implementar tokens CSRF, validar cabeceras Origin/Referer, cookies SameSite.</t>
-  </si>
-  <si>
     <t>Abierto</t>
   </si>
   <si>
@@ -81,30 +65,15 @@
     <t>Crítico (4)</t>
   </si>
   <si>
-    <t>Usar HSTS, pinning de certificados, reforzar TLS 1.3.</t>
-  </si>
-  <si>
-    <t>Intercepción del código de autorización durante la redirección OAuth2.</t>
-  </si>
-  <si>
-    <t>Enforce PKCE, validar state parameter, usar timeouts cortos.</t>
-  </si>
-  <si>
     <t>Exposición de tokens en respuestas HTTP.</t>
   </si>
   <si>
     <t>Ocasional (3)</t>
   </si>
   <si>
-    <t>Usar JWE, cabeceras seguras, token binding.</t>
-  </si>
-  <si>
     <t>Inyección de tokens maliciosos en respuestas HTTP.</t>
   </si>
   <si>
-    <t>Validación de firmas, claims y encabezados.</t>
-  </si>
-  <si>
     <t>Forzar uso de versiones antiguas de SSL/TLS con vulnerabilidades conocidas.</t>
   </si>
   <si>
@@ -114,27 +83,6 @@
     <t>Fuga de información de políticas de autorización a través de consultas en cache.</t>
   </si>
   <si>
-    <t>Encriptación de datos en caché, TTL dinámico, segmentación de datos sensibles.</t>
-  </si>
-  <si>
-    <t>Exposición de jerarquías de roles en respuestas de consulta.</t>
-  </si>
-  <si>
-    <t>Jerarquías planas en caché, enmascaramiento de roles, sanitización de respuestas.</t>
-  </si>
-  <si>
-    <t>Exposición de asignaciones de permisos durante operaciones CRUD.</t>
-  </si>
-  <si>
-    <t>Filtrado de respuestas, logs sanitizados, encriptación en tránsito.</t>
-  </si>
-  <si>
-    <t>Exposición del estado de autorización en consultas.</t>
-  </si>
-  <si>
-    <t>Encriptación de datos, capas de abstracción, filtrado de resultados.</t>
-  </si>
-  <si>
     <t>Exposición de información sensible en claims no esenciales del JWT.</t>
   </si>
   <si>
@@ -201,9 +149,6 @@
     <t>Saturación de los recursos del sistema para interrumpir su funcionamiento.</t>
   </si>
   <si>
-    <t>Implementación de rate limiting, protección anti-DDoS.</t>
-  </si>
-  <si>
     <t>Inyección de Comandos</t>
   </si>
   <si>
@@ -234,9 +179,6 @@
     <t>Ataque de Hombre en el Medio (MITM)</t>
   </si>
   <si>
-    <t>Intercepción de Código de Autorización</t>
-  </si>
-  <si>
     <t>Divulgación de Token</t>
   </si>
   <si>
@@ -249,15 +191,6 @@
     <t>Fuga de Información de la Política de Caché</t>
   </si>
   <si>
-    <t>Divulgación de la Jerarquía de Roles</t>
-  </si>
-  <si>
-    <t>Divulgación de Asignación de Permisos</t>
-  </si>
-  <si>
-    <t>Divulgación del Estado de Autorización</t>
-  </si>
-  <si>
     <t>Divulgación de Reclamaciones Sensibles</t>
   </si>
   <si>
@@ -280,6 +213,24 @@
   </si>
   <si>
     <t>Logging cifrado, versionado de políticas.</t>
+  </si>
+  <si>
+    <t>Agregar tokens simples para evitar solicitudes no autorizadas.</t>
+  </si>
+  <si>
+    <t>Usar HSTS en el servidor, asegurarse de que todas las comunicaciones se realicen a través de HTTPS.</t>
+  </si>
+  <si>
+    <t>Asegurarse de que los tokens estén encriptados y que solo sean enviados a través de conexiones HTTPS. Se hará uso de JWTpara encriptación de tokens.</t>
+  </si>
+  <si>
+    <t>Validar entradas de datos y asegurarse de que sean confiables. Esto usando middlewares como express-jwt.</t>
+  </si>
+  <si>
+    <t>Encriptación de datos en caché y aplicación de un TTL para estos mismos datos.</t>
+  </si>
+  <si>
+    <t>Implementación de rate limiting, configurar límites en el número de solicitudes por usuario o IP en un periodo de tiempo</t>
   </si>
 </sst>
 </file>
@@ -679,10 +630,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -728,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>8</v>
@@ -743,11 +694,11 @@
         <f>IFERROR(VLOOKUP(D2,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E2,Referencias!A$2:B$12,2,FALSE), 0)</f>
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>11</v>
+      <c r="G2" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -755,67 +706,67 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="6">
         <f>IFERROR(VLOOKUP(D3,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E3,Referencias!A$2:B$12,2,FALSE), 0)</f>
         <v>16</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F4" s="6">
         <f>IFERROR(VLOOKUP(D4,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E4,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>16</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>10</v>
@@ -825,10 +776,10 @@
         <v>9</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -836,80 +787,80 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6">
         <f>IFERROR(VLOOKUP(D6,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E6,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6">
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" s="6">
         <f>IFERROR(VLOOKUP(D7,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E7,Referencias!A$2:B$12,2,FALSE), 0)</f>
         <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6">
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F8" s="6">
         <f>IFERROR(VLOOKUP(D8,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E8,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -917,26 +868,26 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F9" s="6">
         <f>IFERROR(VLOOKUP(D9,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E9,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -944,26 +895,26 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="F10" s="6">
         <f>IFERROR(VLOOKUP(D10,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E10,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -971,26 +922,26 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F11" s="6">
         <f>IFERROR(VLOOKUP(D11,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E11,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -998,277 +949,169 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F12" s="6">
         <f>IFERROR(VLOOKUP(D12,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E12,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="F13" s="6">
         <f>IFERROR(VLOOKUP(D13,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E13,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="6">
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>76</v>
+        <v>34</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="F14" s="6">
         <f>IFERROR(VLOOKUP(D14,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E14,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>10</v>
+        <v>38</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="F15" s="6">
         <f>IFERROR(VLOOKUP(D15,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E15,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="H15" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="6">
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>10</v>
+        <v>41</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="F16" s="6">
         <f>IFERROR(VLOOKUP(D16,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E16,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" s="6" t="s">
-        <v>12</v>
+        <v>69</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>79</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F17" s="6">
         <f>IFERROR(VLOOKUP(D17,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E17,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F18" s="6">
-        <f>IFERROR(VLOOKUP(D18,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E18,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>16</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="7">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="6">
-        <f>IFERROR(VLOOKUP(D19,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E19,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>20</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="6">
-        <f>IFERROR(VLOOKUP(D20,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E20,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>16</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="6">
-        <f>IFERROR(VLOOKUP(D21,Referencias!A$8:B$12,2,FALSE), 0)*IFERROR(VLOOKUP(E21,Referencias!A$2:B$12,2,FALSE), 0)</f>
-        <v>12</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="D22:D100" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="D18:D96" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"1 - Improbable,2 - Remoto,3 - Ocasional,4 - Probable,5 - Frecuente"</formula1>
     </dataValidation>
-    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="E22:E100" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="E18:E96" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1 - Bajo,2 - Moderado,3 - Alto,4 - Crítico,5 - Catastrófico"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1280,13 +1123,13 @@
           <x14:formula1>
             <xm:f>Referencias!$A$8:$A$12</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D21</xm:sqref>
+          <xm:sqref>D2:D17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{46565439-40FB-476D-B34B-DE2CD31D6D84}">
           <x14:formula1>
             <xm:f>Referencias!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E21</xm:sqref>
+          <xm:sqref>E2:E17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1310,15 +1153,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1326,7 +1169,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1342,7 +1185,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1350,7 +1193,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1358,15 +1201,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1374,7 +1217,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -1382,7 +1225,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -1398,7 +1241,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>5</v>

</xml_diff>